<commit_message>
Updated and verified category 1, 2, and 5 test cases after implementing the TZ_NAME validation
</commit_message>
<xml_diff>
--- a/docs/packages/CDVM/test cases/CDVM Test Cases.xlsx
+++ b/docs/packages/CDVM/test cases/CDVM Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Category 1 DVM Tests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="309">
   <si>
     <t>Extra Notes</t>
   </si>
@@ -1181,7 +1181,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,12 +1206,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1226,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1327,13 +1321,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1643,8 +1630,8 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54:D54"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" activeCellId="2" sqref="A16:XFD16 A33:XFD33 A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,18 +1869,16 @@
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>80</v>
+      <c r="B16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>305</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>2</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1903,10 +1888,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>2</v>
@@ -1916,14 +1901,14 @@
       <c r="A18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>40</v>
+      <c r="B18" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>2</v>
@@ -1931,29 +1916,33 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10" t="s">
-        <v>67</v>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1961,61 +1950,59 @@
       <c r="A21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E24" s="8"/>
     </row>
@@ -2023,14 +2010,14 @@
       <c r="A25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>46</v>
+      <c r="B25" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" s="8"/>
     </row>
@@ -2041,131 +2028,129 @@
       <c r="B26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>296</v>
+      <c r="C26" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>295</v>
+        <v>29</v>
       </c>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>52</v>
+        <v>303</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>14</v>
+        <v>305</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>54</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>296</v>
+      <c r="A34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>295</v>
+        <v>29</v>
       </c>
       <c r="E34" s="8"/>
     </row>
@@ -2173,31 +2158,37 @@
       <c r="A35" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10" t="s">
-        <v>67</v>
+      <c r="B35" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>296</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>71</v>
+        <v>295</v>
       </c>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
@@ -2209,45 +2200,43 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="B40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>295</v>
       </c>
       <c r="E40" s="8"/>
     </row>
@@ -2255,29 +2244,27 @@
       <c r="A41" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>76</v>
+      <c r="B41" s="8" t="s">
+        <v>302</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>69</v>
+        <v>305</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="8"/>
+        <v>304</v>
+      </c>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="B42" s="9"/>
       <c r="C42" s="11" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E42" s="8"/>
     </row>
@@ -2285,151 +2272,151 @@
       <c r="A43" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>80</v>
+      <c r="B43" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>296</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>2</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>64</v>
+        <v>48</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>66</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B47" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C48" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10" t="s">
+      <c r="B50" s="9"/>
+      <c r="C50" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>81</v>
+        <v>18</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>37</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>82</v>
+        <v>18</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="E52" s="8"/>
     </row>
@@ -2437,61 +2424,61 @@
       <c r="A53" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="13"/>
+      <c r="C53" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C56" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D54" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="E54" s="40"/>
-    </row>
-    <row r="55" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D55" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="E55" s="40"/>
-    </row>
-    <row r="56" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>303</v>
-      </c>
-      <c r="C56" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D56" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="E56" s="40"/>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
@@ -4265,10 +4252,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,28 +4375,30 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -4417,44 +4406,42 @@
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="E12" s="8"/>
     </row>
@@ -4466,216 +4453,261 @@
         <v>44</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="10" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="11" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="10" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>305</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>14</v>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="10" t="s">
+      <c r="B28" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="10" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E30" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5482,8 +5514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5802,24 +5834,21 @@
         <v>209</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>6</v>
+        <v>308</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>235</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>6</v>
@@ -5833,10 +5862,10 @@
     </row>
     <row r="24" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>6</v>
@@ -5844,16 +5873,16 @@
       <c r="D24" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>232</v>
+      <c r="E24" s="37" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>6</v>
@@ -5867,10 +5896,10 @@
     </row>
     <row r="26" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>6</v>
@@ -5879,7 +5908,7 @@
         <v>22</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5901,10 +5930,10 @@
     </row>
     <row r="28" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>6</v>
@@ -5921,7 +5950,7 @@
         <v>214</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>6</v>
@@ -5935,10 +5964,10 @@
     </row>
     <row r="30" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>6</v>
@@ -5947,7 +5976,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5957,22 +5986,19 @@
       <c r="B31" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C31" s="30" t="s">
-        <v>6</v>
+      <c r="C31" s="32" t="s">
+        <v>305</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>6</v>
@@ -5986,10 +6012,10 @@
     </row>
     <row r="33" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>6</v>
@@ -6009,21 +6035,21 @@
         <v>217</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>6</v>
@@ -6032,83 +6058,80 @@
         <v>22</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C36" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="32" t="s">
+      <c r="D38" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E38" s="30" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>22</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>1</v>
+      <c r="A40" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>206</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>1</v>
@@ -6117,15 +6140,15 @@
         <v>1</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>1</v>
+      <c r="A41" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>201</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>1</v>
@@ -6134,7 +6157,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -6142,97 +6165,106 @@
         <v>215</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>295</v>
+        <v>216</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>224</v>
+        <v>52</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>222</v>
-      </c>
-      <c r="C43" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>295</v>
+        <v>1</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="30" t="s">
         <v>300</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B48" s="30" t="s">
         <v>301</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C48" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="D44" s="32" t="s">
+      <c r="D48" s="32" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
-        <v>307</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="B46" s="39" t="s">
-        <v>308</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="B47" s="39" t="s">
-        <v>219</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="B48" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="C48" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CDVM verification bug fix
</commit_message>
<xml_diff>
--- a/docs/packages/CDVM/test cases/CDVM Test Cases.xlsx
+++ b/docs/packages/CDVM/test cases/CDVM Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="14100" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Category 1 DVM Tests" sheetId="1" r:id="rId1"/>
@@ -679,24 +679,6 @@
 completed test case for ORA-20234</t>
   </si>
   <si>
-    <t>executing test case for ORA-20235
-DVM_PKG error: The parent record could not be validated successfully:
-ORA-20219: The data QC validation rules could not be processed for the specified parent record:
-ORA-20235: The validation rule (Mismatched Cruise Name and Fiscal Year) indicator field (CRUISE_ID) has an invalid data type in the data QC view (CCD_QC_CRUISE_V), the DVM requires a character data type for indicator fields:
-ORA-06562: type of out argument must match type of column or bind variable
-The parent record was NOT evaluated successfully
-completed test case for ORA-20235</t>
-  </si>
-  <si>
-    <t>executing test case for ORA-20235
-DVM_PKG error: The parent record could not be validated successfully:
-ORA-20219: The data QC validation rules could not be processed for the specified parent record:
-ORA-20235: The validation rule (Invalid Leg Dates) indicator field (CRUISE_LEG_ID) has an invalid data type in the data QC view (CCD_QC_LEG_V), the DVM requires a character data type for indicator fields:
-ORA-06562: type of out argument must match type of column or bind variable
-The parent record was NOT evaluated successfully
-completed test case for ORA-20235</t>
-  </si>
-  <si>
     <t>Data QC View Does not Contain the Parent Table Primary Key Field</t>
   </si>
   <si>
@@ -1136,6 +1118,24 @@
   </si>
   <si>
     <t>Child records exist</t>
+  </si>
+  <si>
+    <t>executing test case for ORA-20235
+ORA-20237: The parent record could not be validated successfully:
+ORA-20219: The data QC validation rules could not be processed for the specified parent record:
+ORA-20235: The validation rule (Mismatched Cruise Name and Fiscal Year) indicator field (CRUISE_ID) has an invalid data type in the data QC view (CCD_QC_CRUISE_V), the DVM requires a character data type for indicator fields:
+ORA-06562: type of out argument must match type of column or bind variable
+The parent record was NOT evaluated successfully
+completed test case for ORA-20235</t>
+  </si>
+  <si>
+    <t>executing test case for ORA-20235
+ORA-20237: The parent record could not be validated successfully:
+ORA-20219: The data QC validation rules could not be processed for the specified parent record:
+ORA-20235: The validation rule (Invalid Leg Dates) indicator field (CRUISE_LEG_ID) has an invalid data type in the data QC view (CCD_QC_LEG_V), the DVM requires a character data type for indicator fields:
+ORA-06562: type of out argument must match type of column or bind variable
+The parent record was NOT evaluated successfully
+completed test case for ORA-20235</t>
   </si>
 </sst>
 </file>
@@ -1876,10 +1876,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E16" s="11"/>
     </row>
@@ -2047,10 +2047,10 @@
         <v>46</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E27" s="8"/>
     </row>
@@ -2132,13 +2132,13 @@
         <v>34</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>305</v>
-      </c>
       <c r="D33" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -2182,10 +2182,10 @@
         <v>52</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E36" s="8"/>
     </row>
@@ -2248,13 +2248,13 @@
         <v>48</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>304</v>
       </c>
       <c r="E41" s="11"/>
     </row>
@@ -2276,13 +2276,13 @@
         <v>48</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E43" s="8"/>
     </row>
@@ -2473,13 +2473,13 @@
         <v>36</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E56" s="8"/>
     </row>
@@ -3777,7 +3777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -3792,7 +3792,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>107</v>
@@ -3809,16 +3809,16 @@
     </row>
     <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>246</v>
-      </c>
       <c r="D2" s="27" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E2" s="2">
         <v>-20501</v>
@@ -3829,13 +3829,13 @@
         <v>-1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>247</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>249</v>
       </c>
       <c r="E3">
         <v>-20502</v>
@@ -3843,16 +3843,16 @@
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C4" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>248</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>250</v>
       </c>
       <c r="E4" s="2">
         <v>-20501</v>
@@ -3860,16 +3860,16 @@
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E5">
         <v>-20502</v>
@@ -3877,16 +3877,16 @@
     </row>
     <row r="6" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E6">
         <v>-20505</v>
@@ -3894,16 +3894,16 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E7">
         <v>-20507</v>
@@ -3914,13 +3914,13 @@
         <v>-1</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E8">
         <v>-20508</v>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E9">
         <v>-20507</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E10">
         <v>-20509</v>
@@ -3962,16 +3962,16 @@
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E11">
         <v>-20510</v>
@@ -3982,13 +3982,13 @@
         <v>-1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E12">
         <v>-20511</v>
@@ -3996,16 +3996,16 @@
     </row>
     <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E13">
         <v>-20510</v>
@@ -4013,16 +4013,16 @@
     </row>
     <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E14">
         <v>-20512</v>
@@ -4030,16 +4030,16 @@
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E15" s="2">
         <v>-20513</v>
@@ -4047,16 +4047,16 @@
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E16" s="2">
         <v>-20513</v>
@@ -4067,13 +4067,13 @@
         <v>-1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E17" s="2">
         <v>-20515</v>
@@ -4081,16 +4081,16 @@
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E18" s="2">
         <v>-20515</v>
@@ -4101,13 +4101,13 @@
         <v>41</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E19" s="2">
         <v>-20516</v>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E20" s="2">
         <v>-20517</v>
@@ -4132,16 +4132,16 @@
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E21" s="2">
         <v>-20517</v>
@@ -4152,13 +4152,13 @@
         <v>-1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E22" s="2">
         <v>-20519</v>
@@ -4166,16 +4166,16 @@
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E23" s="2">
         <v>-20519</v>
@@ -4183,16 +4183,16 @@
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E24" s="2">
         <v>-20520</v>
@@ -4200,16 +4200,16 @@
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E25" s="2">
         <v>-20520</v>
@@ -4220,13 +4220,13 @@
         <v>-1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E26" s="2">
         <v>-20522</v>
@@ -4234,16 +4234,16 @@
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E27" s="2">
         <v>-20522</v>
@@ -4387,10 +4387,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E8" s="11"/>
     </row>
@@ -4511,13 +4511,13 @@
         <v>34</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>305</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E17" s="11"/>
     </row>
@@ -4567,13 +4567,13 @@
         <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>304</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -5181,8 +5181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5475,7 +5475,7 @@
         <v>189</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>191</v>
+        <v>308</v>
       </c>
       <c r="E18" s="2">
         <v>-20235</v>
@@ -5489,7 +5489,7 @@
         <v>189</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>192</v>
+        <v>309</v>
       </c>
       <c r="E19" s="2">
         <v>-20235</v>
@@ -5497,13 +5497,13 @@
     </row>
     <row r="20" spans="2:5" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E20" s="2">
         <v>-20236</v>
@@ -5572,7 +5572,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5629,7 +5629,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5697,10 +5697,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5771,7 +5771,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5800,7 +5800,7 @@
         <v>21</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5817,7 +5817,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -5836,24 +5836,24 @@
     </row>
     <row r="22" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>6</v>
@@ -5862,15 +5862,15 @@
         <v>22</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>6</v>
@@ -5879,15 +5879,15 @@
         <v>22</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>6</v>
@@ -5896,15 +5896,15 @@
         <v>22</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>6</v>
@@ -5913,15 +5913,15 @@
         <v>22</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>6</v>
@@ -5930,15 +5930,15 @@
         <v>22</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>6</v>
@@ -5947,15 +5947,15 @@
         <v>22</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>6</v>
@@ -5964,15 +5964,15 @@
         <v>22</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>6</v>
@@ -5981,29 +5981,29 @@
         <v>22</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>6</v>
@@ -6012,15 +6012,15 @@
         <v>22</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>6</v>
@@ -6029,15 +6029,15 @@
         <v>22</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>6</v>
@@ -6046,15 +6046,15 @@
         <v>22</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>6</v>
@@ -6063,15 +6063,15 @@
         <v>22</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>82</v>
@@ -6080,29 +6080,29 @@
         <v>29</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="30" t="s">
         <v>223</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>225</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>6</v>
@@ -6111,15 +6111,15 @@
         <v>22</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C39" s="30" t="s">
         <v>6</v>
@@ -6128,15 +6128,15 @@
         <v>22</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>1</v>
@@ -6145,15 +6145,15 @@
         <v>1</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>1</v>
@@ -6162,15 +6162,15 @@
         <v>1</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C42" s="30" t="s">
         <v>1</v>
@@ -6179,7 +6179,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -6196,7 +6196,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -6213,63 +6213,63 @@
         <v>1</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B46" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="C46" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -8817,10 +8817,10 @@
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -8969,18 +8969,18 @@
     </row>
     <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="28" t="s">
         <v>196</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>